<commit_message>
Zapytania o ogloszenia po froncie
</commit_message>
<xml_diff>
--- a/Projekt 2 - sprzątando + admin panel.xlsx
+++ b/Projekt 2 - sprzątando + admin panel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Aktualne projekty\Szkoła Sprzatando\Sprzatando\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projekty\Web\sprzatando\Sprzatando\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8426797E-AB1F-4F4D-B3A7-F11095546182}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{494B8121-328C-41E8-B672-AEE44C452334}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -618,7 +618,7 @@
   <dimension ref="A1:G41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -688,7 +688,7 @@
       </c>
       <c r="E7" s="7">
         <f>COUNTIF(C:C, TRUE)</f>
-        <v>8</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -724,7 +724,7 @@
       </c>
       <c r="E11" s="8">
         <f>E7*100/E3</f>
-        <v>32</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -740,7 +740,7 @@
         <v>15</v>
       </c>
       <c r="C13" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E13" s="8" t="s">
         <v>16</v>
@@ -835,7 +835,7 @@
         <v>29</v>
       </c>
       <c r="C21" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -843,7 +843,7 @@
         <v>30</v>
       </c>
       <c r="C22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -851,7 +851,7 @@
         <v>31</v>
       </c>
       <c r="C23" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -859,7 +859,7 @@
         <v>32</v>
       </c>
       <c r="C24" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -867,7 +867,7 @@
         <v>33</v>
       </c>
       <c r="C25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -875,7 +875,7 @@
         <v>34</v>
       </c>
       <c r="C26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -883,7 +883,7 @@
         <v>35</v>
       </c>
       <c r="C27" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -891,7 +891,7 @@
         <v>36</v>
       </c>
       <c r="C28" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -975,9 +975,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1113,19 +1116,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{93A548D2-ECF0-4E52-A77F-2150500620BD}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC939A35-43C5-42BD-B567-14742099AD82}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1149,9 +1148,10 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC939A35-43C5-42BD-B567-14742099AD82}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{93A548D2-ECF0-4E52-A77F-2150500620BD}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>